<commit_message>
"- ส่วนของ Advance Search ตัดพารามิเตอร์ Department, Section ออก และเพิ่มพารามิเตอร์ Organization แสดงเป็น Select Search - ส่วนของ List ตัด Field Department, Section ออก และเพิ่ม Field Organization - ส่วนของ Edit ตัด Field Department Code, Department Name, Section Code, Section Name, Position Code, Position Name, Position Group และเพิ่ม Field Organization แสดงเป็น Dropdown และ Position แสดงเป็น Select Search - ส่วนของ Download/Import Tamplate ตัด Field และเพิ่ม Field เหมือนกับส่วนของ Edit"
</commit_message>
<xml_diff>
--- a/docroot/file/import_employee_template.xlsx
+++ b/docroot/file/import_employee_template.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18229"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Employee Code</t>
   </si>
@@ -41,33 +41,9 @@
     <t>Acting End Date (YYYY-MM-DD)</t>
   </si>
   <si>
-    <t>Department Code</t>
-  </si>
-  <si>
-    <t>Department Name</t>
-  </si>
-  <si>
-    <t>Section Code</t>
-  </si>
-  <si>
-    <t>Section Name</t>
-  </si>
-  <si>
-    <t>Position Code</t>
-  </si>
-  <si>
-    <t>Position Name</t>
-  </si>
-  <si>
-    <t>Position Group</t>
-  </si>
-  <si>
     <t>Salary Amount</t>
   </si>
   <si>
-    <t>ERP User</t>
-  </si>
-  <si>
     <t>Employee Type</t>
   </si>
   <si>
@@ -75,6 +51,15 @@
   </si>
   <si>
     <t>Chief Employee Code</t>
+  </si>
+  <si>
+    <t>Org ID</t>
+  </si>
+  <si>
+    <t>Position ID</t>
+  </si>
+  <si>
+    <t>Level ID</t>
   </si>
 </sst>
 </file>
@@ -442,36 +427,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q1"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.42578125" style="2"/>
     <col min="2" max="2" width="34.42578125" style="2"/>
-    <col min="3" max="3" width="29.42578125" style="4"/>
-    <col min="4" max="4" width="29.7109375" style="4"/>
-    <col min="5" max="5" width="27.140625" style="4"/>
+    <col min="3" max="3" width="33" style="4" customWidth="1"/>
+    <col min="4" max="4" width="31.85546875" style="4" customWidth="1"/>
+    <col min="5" max="5" width="29.5703125" style="4" customWidth="1"/>
     <col min="6" max="6" width="16.42578125" style="2"/>
-    <col min="7" max="7" width="20.28515625" style="2"/>
-    <col min="8" max="8" width="12.5703125" style="2"/>
-    <col min="9" max="9" width="29.7109375" style="2"/>
-    <col min="10" max="10" width="13.140625" style="2"/>
-    <col min="11" max="11" width="32.42578125" style="2"/>
-    <col min="12" max="12" width="13.7109375" style="2"/>
-    <col min="13" max="13" width="23.85546875" style="2"/>
-    <col min="14" max="14" width="13.7109375" style="2"/>
-    <col min="15" max="15" width="8.7109375" style="2"/>
-    <col min="16" max="16" width="14" style="2"/>
-    <col min="17" max="17" width="23.7109375" style="2"/>
-    <col min="18" max="1005" width="11.28515625" style="2"/>
-    <col min="1006" max="16384" width="8.85546875" style="2"/>
+    <col min="7" max="7" width="13.140625" style="2"/>
+    <col min="8" max="8" width="23.85546875" style="2"/>
+    <col min="9" max="9" width="8.85546875" style="2"/>
+    <col min="10" max="10" width="13.7109375" style="2"/>
+    <col min="11" max="11" width="24.85546875" style="2" customWidth="1"/>
+    <col min="12" max="12" width="14" style="2"/>
+    <col min="13" max="13" width="23.7109375" style="2"/>
+    <col min="14" max="1001" width="11.28515625" style="2"/>
+    <col min="1002" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -488,44 +469,30 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="K1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="M1" s="1"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
+  <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="portrait" useFirstPageNumber="1" r:id="rId1"/>
   <headerFooter>

</xml_diff>